<commit_message>
Deletado alguns arquivos de segmentação
</commit_message>
<xml_diff>
--- a/Base/metadadosdrogas.xlsx
+++ b/Base/metadadosdrogas.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -4106,7 +4106,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4120,9 +4120,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4160,7 +4160,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -4232,7 +4232,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4408,8 +4408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A959" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G1001" sqref="G1001"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>